<commit_message>
Implementado delilimatador de mapa para el Agente
</commit_message>
<xml_diff>
--- a/mapfiles/template_maps.xlsx
+++ b/mapfiles/template_maps.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="40">
   <si>
     <t>1</t>
   </si>
@@ -67,6 +67,75 @@
   <si>
     <t>O</t>
   </si>
+  <si>
+    <t>z,x</t>
+  </si>
+  <si>
+    <t>0,15</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>0,5</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>15,0</t>
+  </si>
+  <si>
+    <t>15,8</t>
+  </si>
+  <si>
+    <t>14,8</t>
+  </si>
+  <si>
+    <t>13,8</t>
+  </si>
+  <si>
+    <t>12,8</t>
+  </si>
+  <si>
+    <t>11,8</t>
+  </si>
+  <si>
+    <t>10,8</t>
+  </si>
+  <si>
+    <t>9,8</t>
+  </si>
+  <si>
+    <t>8,8</t>
+  </si>
+  <si>
+    <t>8,6</t>
+  </si>
+  <si>
+    <t>8,7</t>
+  </si>
+  <si>
+    <t>8,5</t>
+  </si>
+  <si>
+    <t>7,5</t>
+  </si>
+  <si>
+    <t>6,5</t>
+  </si>
+  <si>
+    <t>5,5</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>3,5</t>
+  </si>
 </sst>
 </file>
 
@@ -101,9 +170,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,15 +478,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ36"/>
+  <dimension ref="A1:AM41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="5.140625" style="1"/>
+    <col min="1" max="38" width="5.140625" style="1"/>
+    <col min="39" max="39" width="5.140625" style="2"/>
+    <col min="40" max="16384" width="5.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -468,6 +540,9 @@
       <c r="Q1" s="1">
         <v>15</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
@@ -522,67 +597,67 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f>$A2  &amp; "," &amp; B$1</f>
+        <f t="shared" ref="B2:B17" si="0">$A2  &amp; "," &amp; B$1</f>
         <v>15,0</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:Q17" si="0">$A2  &amp; "," &amp; C$1</f>
+        <f t="shared" ref="C2:Q17" si="1">$A2  &amp; "," &amp; C$1</f>
         <v>15,1</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,2</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,3</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,4</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,5</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,6</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,7</v>
       </c>
       <c r="J2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,8</v>
       </c>
       <c r="K2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,9</v>
       </c>
       <c r="L2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,10</v>
       </c>
       <c r="M2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,11</v>
       </c>
       <c r="N2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,12</v>
       </c>
       <c r="O2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,13</v>
       </c>
       <c r="P2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,14</v>
       </c>
       <c r="Q2" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15,15</v>
       </c>
       <c r="T2" s="1">
@@ -642,67 +717,67 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>14,0</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; C$1</f>
+        <f t="shared" ref="C3:P17" si="2">$A3  &amp; "," &amp; C$1</f>
         <v>14,1</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>14,2</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>14,3</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>14,4</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>14,5</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>14,6</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>14,7</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>14,8</v>
       </c>
       <c r="K3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>14,9</v>
       </c>
       <c r="L3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>14,10</v>
       </c>
       <c r="M3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>14,11</v>
       </c>
       <c r="N3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>14,12</v>
       </c>
       <c r="O3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>14,13</v>
       </c>
       <c r="P3" s="1" t="str">
-        <f>$A3  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>14,14</v>
       </c>
       <c r="Q3" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14,15</v>
       </c>
       <c r="T3" s="1">
@@ -762,67 +837,67 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>13,0</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>13,1</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>13,2</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>13,3</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>13,4</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>13,5</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>13,6</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>13,7</v>
       </c>
       <c r="J4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>13,8</v>
       </c>
       <c r="K4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>13,9</v>
       </c>
       <c r="L4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>13,10</v>
       </c>
       <c r="M4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>13,11</v>
       </c>
       <c r="N4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>13,12</v>
       </c>
       <c r="O4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>13,13</v>
       </c>
       <c r="P4" s="1" t="str">
-        <f>$A4  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>13,14</v>
       </c>
       <c r="Q4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13,15</v>
       </c>
       <c r="T4" s="1">
@@ -882,67 +957,67 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>12,0</v>
       </c>
       <c r="C5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>12,1</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>12,2</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>12,3</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>12,4</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>12,5</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>12,6</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>12,7</v>
       </c>
       <c r="J5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>12,8</v>
       </c>
       <c r="K5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>12,9</v>
       </c>
       <c r="L5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>12,10</v>
       </c>
       <c r="M5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>12,11</v>
       </c>
       <c r="N5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>12,12</v>
       </c>
       <c r="O5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>12,13</v>
       </c>
       <c r="P5" s="1" t="str">
-        <f>$A5  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>12,14</v>
       </c>
       <c r="Q5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12,15</v>
       </c>
       <c r="T5" s="1">
@@ -1002,67 +1077,67 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>11,0</v>
       </c>
       <c r="C6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>11,1</v>
       </c>
       <c r="D6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>11,2</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>11,3</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>11,4</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>11,5</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>11,6</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>11,7</v>
       </c>
       <c r="J6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>11,8</v>
       </c>
       <c r="K6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>11,9</v>
       </c>
       <c r="L6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>11,10</v>
       </c>
       <c r="M6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>11,11</v>
       </c>
       <c r="N6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>11,12</v>
       </c>
       <c r="O6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>11,13</v>
       </c>
       <c r="P6" s="1" t="str">
-        <f>$A6  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>11,14</v>
       </c>
       <c r="Q6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11,15</v>
       </c>
       <c r="T6" s="1">
@@ -1122,67 +1197,67 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>10,0</v>
       </c>
       <c r="C7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>10,1</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>10,2</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>10,3</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>10,4</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>10,5</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>10,6</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>10,7</v>
       </c>
       <c r="J7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>10,8</v>
       </c>
       <c r="K7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>10,9</v>
       </c>
       <c r="L7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>10,10</v>
       </c>
       <c r="M7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>10,11</v>
       </c>
       <c r="N7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>10,12</v>
       </c>
       <c r="O7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>10,13</v>
       </c>
       <c r="P7" s="1" t="str">
-        <f>$A7  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>10,14</v>
       </c>
       <c r="Q7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10,15</v>
       </c>
       <c r="T7" s="1">
@@ -1242,67 +1317,67 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>9,0</v>
       </c>
       <c r="C8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>9,1</v>
       </c>
       <c r="D8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>9,2</v>
       </c>
       <c r="E8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>9,3</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>9,4</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>9,5</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>9,6</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>9,7</v>
       </c>
       <c r="J8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>9,8</v>
       </c>
       <c r="K8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>9,9</v>
       </c>
       <c r="L8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>9,10</v>
       </c>
       <c r="M8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>9,11</v>
       </c>
       <c r="N8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>9,12</v>
       </c>
       <c r="O8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>9,13</v>
       </c>
       <c r="P8" s="1" t="str">
-        <f>$A8  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>9,14</v>
       </c>
       <c r="Q8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9,15</v>
       </c>
       <c r="T8" s="1">
@@ -1362,67 +1437,67 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>8,0</v>
       </c>
       <c r="C9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>8,1</v>
       </c>
       <c r="D9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>8,2</v>
       </c>
       <c r="E9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>8,3</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>8,4</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>8,5</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>8,6</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>8,7</v>
       </c>
       <c r="J9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>8,8</v>
       </c>
       <c r="K9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>8,9</v>
       </c>
       <c r="L9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>8,10</v>
       </c>
       <c r="M9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>8,11</v>
       </c>
       <c r="N9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>8,12</v>
       </c>
       <c r="O9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>8,13</v>
       </c>
       <c r="P9" s="1" t="str">
-        <f>$A9  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>8,14</v>
       </c>
       <c r="Q9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8,15</v>
       </c>
       <c r="T9" s="1">
@@ -1482,67 +1557,67 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>7,0</v>
       </c>
       <c r="C10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>7,1</v>
       </c>
       <c r="D10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>7,2</v>
       </c>
       <c r="E10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>7,3</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>7,4</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>7,5</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>7,6</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>7,7</v>
       </c>
       <c r="J10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>7,8</v>
       </c>
       <c r="K10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>7,9</v>
       </c>
       <c r="L10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>7,10</v>
       </c>
       <c r="M10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>7,11</v>
       </c>
       <c r="N10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>7,12</v>
       </c>
       <c r="O10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>7,13</v>
       </c>
       <c r="P10" s="1" t="str">
-        <f>$A10  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>7,14</v>
       </c>
       <c r="Q10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7,15</v>
       </c>
       <c r="T10" s="1">
@@ -1602,67 +1677,67 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>6,0</v>
       </c>
       <c r="C11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>6,1</v>
       </c>
       <c r="D11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>6,2</v>
       </c>
       <c r="E11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>6,3</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>6,4</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>6,5</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>6,6</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>6,7</v>
       </c>
       <c r="J11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>6,8</v>
       </c>
       <c r="K11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>6,9</v>
       </c>
       <c r="L11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>6,10</v>
       </c>
       <c r="M11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>6,11</v>
       </c>
       <c r="N11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>6,12</v>
       </c>
       <c r="O11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>6,13</v>
       </c>
       <c r="P11" s="1" t="str">
-        <f>$A11  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>6,14</v>
       </c>
       <c r="Q11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6,15</v>
       </c>
       <c r="T11" s="1">
@@ -1722,67 +1797,67 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>5,0</v>
       </c>
       <c r="C12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>5,1</v>
       </c>
       <c r="D12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>5,2</v>
       </c>
       <c r="E12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>5,3</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>5,4</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>5,5</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>5,6</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>5,7</v>
       </c>
       <c r="J12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>5,8</v>
       </c>
       <c r="K12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>5,9</v>
       </c>
       <c r="L12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>5,10</v>
       </c>
       <c r="M12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>5,11</v>
       </c>
       <c r="N12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>5,12</v>
       </c>
       <c r="O12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>5,13</v>
       </c>
       <c r="P12" s="1" t="str">
-        <f>$A12  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>5,14</v>
       </c>
       <c r="Q12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5,15</v>
       </c>
       <c r="T12" s="1">
@@ -1842,67 +1917,67 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>4,0</v>
       </c>
       <c r="C13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>4,1</v>
       </c>
       <c r="D13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>4,2</v>
       </c>
       <c r="E13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>4,3</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>4,4</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>4,5</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>4,6</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>4,7</v>
       </c>
       <c r="J13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>4,8</v>
       </c>
       <c r="K13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>4,9</v>
       </c>
       <c r="L13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>4,10</v>
       </c>
       <c r="M13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>4,11</v>
       </c>
       <c r="N13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>4,12</v>
       </c>
       <c r="O13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>4,13</v>
       </c>
       <c r="P13" s="1" t="str">
-        <f>$A13  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>4,14</v>
       </c>
       <c r="Q13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4,15</v>
       </c>
       <c r="T13" s="1">
@@ -1962,67 +2037,67 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>3,0</v>
       </c>
       <c r="C14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>3,1</v>
       </c>
       <c r="D14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>3,2</v>
       </c>
       <c r="E14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>3,3</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>3,4</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>3,5</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>3,6</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>3,7</v>
       </c>
       <c r="J14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>3,8</v>
       </c>
       <c r="K14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>3,9</v>
       </c>
       <c r="L14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>3,10</v>
       </c>
       <c r="M14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>3,11</v>
       </c>
       <c r="N14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>3,12</v>
       </c>
       <c r="O14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>3,13</v>
       </c>
       <c r="P14" s="1" t="str">
-        <f>$A14  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>3,14</v>
       </c>
       <c r="Q14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3,15</v>
       </c>
       <c r="T14" s="1">
@@ -2082,67 +2157,67 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>2,0</v>
       </c>
       <c r="C15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>2,1</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>2,2</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>2,3</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>2,4</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>2,5</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>2,6</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>2,7</v>
       </c>
       <c r="J15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>2,8</v>
       </c>
       <c r="K15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>2,9</v>
       </c>
       <c r="L15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>2,10</v>
       </c>
       <c r="M15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>2,11</v>
       </c>
       <c r="N15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>2,12</v>
       </c>
       <c r="O15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>2,13</v>
       </c>
       <c r="P15" s="1" t="str">
-        <f>$A15  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>2,14</v>
       </c>
       <c r="Q15" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2,15</v>
       </c>
       <c r="T15" s="1">
@@ -2202,67 +2277,67 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>1,0</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>1,1</v>
       </c>
       <c r="D16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>1,2</v>
       </c>
       <c r="E16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>1,3</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>1,4</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>1,5</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>1,6</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>1,7</v>
       </c>
       <c r="J16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>1,8</v>
       </c>
       <c r="K16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>1,9</v>
       </c>
       <c r="L16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>1,10</v>
       </c>
       <c r="M16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>1,11</v>
       </c>
       <c r="N16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>1,12</v>
       </c>
       <c r="O16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>1,13</v>
       </c>
       <c r="P16" s="1" t="str">
-        <f>$A16  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>1,14</v>
       </c>
       <c r="Q16" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1,15</v>
       </c>
       <c r="T16" s="1">
@@ -2317,72 +2392,72 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; B$1</f>
+        <f t="shared" si="0"/>
         <v>0,0</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; C$1</f>
+        <f t="shared" si="2"/>
         <v>0,1</v>
       </c>
       <c r="D17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; D$1</f>
+        <f t="shared" si="2"/>
         <v>0,2</v>
       </c>
       <c r="E17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; E$1</f>
+        <f t="shared" si="2"/>
         <v>0,3</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; F$1</f>
+        <f t="shared" si="2"/>
         <v>0,4</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; G$1</f>
+        <f t="shared" si="2"/>
         <v>0,5</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; H$1</f>
+        <f t="shared" si="2"/>
         <v>0,6</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; I$1</f>
+        <f t="shared" si="2"/>
         <v>0,7</v>
       </c>
       <c r="J17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; J$1</f>
+        <f t="shared" si="2"/>
         <v>0,8</v>
       </c>
       <c r="K17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; K$1</f>
+        <f t="shared" si="2"/>
         <v>0,9</v>
       </c>
       <c r="L17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; L$1</f>
+        <f t="shared" si="2"/>
         <v>0,10</v>
       </c>
       <c r="M17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; M$1</f>
+        <f t="shared" si="2"/>
         <v>0,11</v>
       </c>
       <c r="N17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; N$1</f>
+        <f t="shared" si="2"/>
         <v>0,12</v>
       </c>
       <c r="O17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; O$1</f>
+        <f t="shared" si="2"/>
         <v>0,13</v>
       </c>
       <c r="P17" s="1" t="str">
-        <f>$A17  &amp; "," &amp; P$1</f>
+        <f t="shared" si="2"/>
         <v>0,14</v>
       </c>
       <c r="Q17" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0,15</v>
       </c>
       <c r="T17" s="1">
@@ -2437,12 +2512,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="AM19" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
@@ -2539,8 +2617,11 @@
       <c r="AJ20" s="1">
         <v>15</v>
       </c>
+      <c r="AM20" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>15</v>
       </c>
@@ -2590,71 +2671,74 @@
         <v>15</v>
       </c>
       <c r="U21" s="1" t="str">
-        <f>IF(B21="O","",B2)</f>
+        <f t="shared" ref="U21:U36" si="3">IF(B21="O","",B2)</f>
         <v>15,0</v>
       </c>
       <c r="V21" s="1" t="str">
-        <f>IF(C21="O","",C2)</f>
+        <f t="shared" ref="V21:V36" si="4">IF(C21="O","",C2)</f>
         <v/>
       </c>
       <c r="W21" s="1" t="str">
-        <f>IF(D21="O","",D2)</f>
+        <f t="shared" ref="W21:W36" si="5">IF(D21="O","",D2)</f>
         <v/>
       </c>
       <c r="X21" s="1" t="str">
-        <f>IF(E21="O","",E2)</f>
+        <f t="shared" ref="X21:X36" si="6">IF(E21="O","",E2)</f>
         <v/>
       </c>
       <c r="Y21" s="1" t="str">
-        <f>IF(F21="O","",F2)</f>
+        <f t="shared" ref="Y21:Y36" si="7">IF(F21="O","",F2)</f>
         <v/>
       </c>
       <c r="Z21" s="1" t="str">
-        <f>IF(G21="O","",G2)</f>
+        <f t="shared" ref="Z21:Z36" si="8">IF(G21="O","",G2)</f>
         <v/>
       </c>
       <c r="AA21" s="1" t="str">
-        <f>IF(H21="O","",H2)</f>
+        <f t="shared" ref="AA21:AA36" si="9">IF(H21="O","",H2)</f>
         <v/>
       </c>
       <c r="AB21" s="1" t="str">
-        <f>IF(I21="O","",I2)</f>
+        <f t="shared" ref="AB21:AB36" si="10">IF(I21="O","",I2)</f>
         <v/>
       </c>
       <c r="AC21" s="1" t="str">
-        <f>IF(J21="O","",J2)</f>
+        <f t="shared" ref="AC21:AC36" si="11">IF(J21="O","",J2)</f>
         <v>15,8</v>
       </c>
       <c r="AD21" s="1" t="str">
-        <f>IF(K21="O","",K2)</f>
+        <f t="shared" ref="AD21:AD36" si="12">IF(K21="O","",K2)</f>
         <v/>
       </c>
       <c r="AE21" s="1" t="str">
-        <f>IF(L21="O","",L2)</f>
+        <f t="shared" ref="AE21:AE36" si="13">IF(L21="O","",L2)</f>
         <v/>
       </c>
       <c r="AF21" s="1" t="str">
-        <f>IF(M21="O","",M2)</f>
+        <f t="shared" ref="AF21:AF36" si="14">IF(M21="O","",M2)</f>
         <v/>
       </c>
       <c r="AG21" s="1" t="str">
-        <f>IF(N21="O","",N2)</f>
+        <f t="shared" ref="AG21:AG36" si="15">IF(N21="O","",N2)</f>
         <v/>
       </c>
       <c r="AH21" s="1" t="str">
-        <f>IF(O21="O","",O2)</f>
+        <f t="shared" ref="AH21:AH36" si="16">IF(O21="O","",O2)</f>
         <v/>
       </c>
       <c r="AI21" s="1" t="str">
-        <f>IF(P21="O","",P2)</f>
+        <f t="shared" ref="AI21:AI36" si="17">IF(P21="O","",P2)</f>
         <v/>
       </c>
       <c r="AJ21" s="1" t="str">
-        <f>IF(Q21="O","",Q2)</f>
-        <v/>
+        <f t="shared" ref="AJ21:AJ36" si="18">IF(Q21="O","",Q2)</f>
+        <v/>
+      </c>
+      <c r="AM21" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>14</v>
       </c>
@@ -2707,71 +2791,74 @@
         <v>14</v>
       </c>
       <c r="U22" s="1" t="str">
-        <f>IF(B22="O","",B3)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V22" s="1" t="str">
-        <f>IF(C22="O","",C3)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W22" s="1" t="str">
-        <f>IF(D22="O","",D3)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X22" s="1" t="str">
-        <f>IF(E22="O","",E3)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y22" s="1" t="str">
-        <f>IF(F22="O","",F3)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z22" s="1" t="str">
-        <f>IF(G22="O","",G3)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AA22" s="1" t="str">
-        <f>IF(H22="O","",H3)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB22" s="1" t="str">
-        <f>IF(I22="O","",I3)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC22" s="1" t="str">
-        <f>IF(J22="O","",J3)</f>
+        <f t="shared" si="11"/>
         <v>14,8</v>
       </c>
       <c r="AD22" s="1" t="str">
-        <f>IF(K22="O","",K3)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE22" s="1" t="str">
-        <f>IF(L22="O","",L3)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF22" s="1" t="str">
-        <f>IF(M22="O","",M3)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG22" s="1" t="str">
-        <f>IF(N22="O","",N3)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH22" s="1" t="str">
-        <f>IF(O22="O","",O3)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI22" s="1" t="str">
-        <f>IF(P22="O","",P3)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ22" s="1" t="str">
-        <f>IF(Q22="O","",Q3)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM22" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>13</v>
       </c>
@@ -2824,71 +2911,74 @@
         <v>13</v>
       </c>
       <c r="U23" s="1" t="str">
-        <f>IF(B23="O","",B4)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V23" s="1" t="str">
-        <f>IF(C23="O","",C4)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W23" s="1" t="str">
-        <f>IF(D23="O","",D4)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X23" s="1" t="str">
-        <f>IF(E23="O","",E4)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y23" s="1" t="str">
-        <f>IF(F23="O","",F4)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z23" s="1" t="str">
-        <f>IF(G23="O","",G4)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AA23" s="1" t="str">
-        <f>IF(H23="O","",H4)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB23" s="1" t="str">
-        <f>IF(I23="O","",I4)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC23" s="1" t="str">
-        <f>IF(J23="O","",J4)</f>
+        <f t="shared" si="11"/>
         <v>13,8</v>
       </c>
       <c r="AD23" s="1" t="str">
-        <f>IF(K23="O","",K4)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE23" s="1" t="str">
-        <f>IF(L23="O","",L4)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF23" s="1" t="str">
-        <f>IF(M23="O","",M4)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG23" s="1" t="str">
-        <f>IF(N23="O","",N4)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH23" s="1" t="str">
-        <f>IF(O23="O","",O4)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI23" s="1" t="str">
-        <f>IF(P23="O","",P4)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ23" s="1" t="str">
-        <f>IF(Q23="O","",Q4)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM23" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>12</v>
       </c>
@@ -2941,71 +3031,74 @@
         <v>12</v>
       </c>
       <c r="U24" s="1" t="str">
-        <f>IF(B24="O","",B5)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V24" s="1" t="str">
-        <f>IF(C24="O","",C5)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W24" s="1" t="str">
-        <f>IF(D24="O","",D5)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X24" s="1" t="str">
-        <f>IF(E24="O","",E5)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y24" s="1" t="str">
-        <f>IF(F24="O","",F5)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z24" s="1" t="str">
-        <f>IF(G24="O","",G5)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AA24" s="1" t="str">
-        <f>IF(H24="O","",H5)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB24" s="1" t="str">
-        <f>IF(I24="O","",I5)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC24" s="1" t="str">
-        <f>IF(J24="O","",J5)</f>
+        <f t="shared" si="11"/>
         <v>12,8</v>
       </c>
       <c r="AD24" s="1" t="str">
-        <f>IF(K24="O","",K5)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE24" s="1" t="str">
-        <f>IF(L24="O","",L5)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF24" s="1" t="str">
-        <f>IF(M24="O","",M5)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG24" s="1" t="str">
-        <f>IF(N24="O","",N5)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH24" s="1" t="str">
-        <f>IF(O24="O","",O5)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI24" s="1" t="str">
-        <f>IF(P24="O","",P5)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ24" s="1" t="str">
-        <f>IF(Q24="O","",Q5)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM24" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>11</v>
       </c>
@@ -3058,71 +3151,74 @@
         <v>11</v>
       </c>
       <c r="U25" s="1" t="str">
-        <f>IF(B25="O","",B6)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V25" s="1" t="str">
-        <f>IF(C25="O","",C6)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W25" s="1" t="str">
-        <f>IF(D25="O","",D6)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X25" s="1" t="str">
-        <f>IF(E25="O","",E6)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y25" s="1" t="str">
-        <f>IF(F25="O","",F6)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z25" s="1" t="str">
-        <f>IF(G25="O","",G6)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AA25" s="1" t="str">
-        <f>IF(H25="O","",H6)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB25" s="1" t="str">
-        <f>IF(I25="O","",I6)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC25" s="1" t="str">
-        <f>IF(J25="O","",J6)</f>
+        <f t="shared" si="11"/>
         <v>11,8</v>
       </c>
       <c r="AD25" s="1" t="str">
-        <f>IF(K25="O","",K6)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE25" s="1" t="str">
-        <f>IF(L25="O","",L6)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF25" s="1" t="str">
-        <f>IF(M25="O","",M6)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG25" s="1" t="str">
-        <f>IF(N25="O","",N6)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH25" s="1" t="str">
-        <f>IF(O25="O","",O6)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI25" s="1" t="str">
-        <f>IF(P25="O","",P6)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ25" s="1" t="str">
-        <f>IF(Q25="O","",Q6)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM25" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>10</v>
       </c>
@@ -3175,71 +3271,74 @@
         <v>10</v>
       </c>
       <c r="U26" s="1" t="str">
-        <f>IF(B26="O","",B7)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V26" s="1" t="str">
-        <f>IF(C26="O","",C7)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W26" s="1" t="str">
-        <f>IF(D26="O","",D7)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X26" s="1" t="str">
-        <f>IF(E26="O","",E7)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y26" s="1" t="str">
-        <f>IF(F26="O","",F7)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z26" s="1" t="str">
-        <f>IF(G26="O","",G7)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AA26" s="1" t="str">
-        <f>IF(H26="O","",H7)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB26" s="1" t="str">
-        <f>IF(I26="O","",I7)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC26" s="1" t="str">
-        <f>IF(J26="O","",J7)</f>
+        <f t="shared" si="11"/>
         <v>10,8</v>
       </c>
       <c r="AD26" s="1" t="str">
-        <f>IF(K26="O","",K7)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE26" s="1" t="str">
-        <f>IF(L26="O","",L7)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF26" s="1" t="str">
-        <f>IF(M26="O","",M7)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG26" s="1" t="str">
-        <f>IF(N26="O","",N7)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH26" s="1" t="str">
-        <f>IF(O26="O","",O7)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI26" s="1" t="str">
-        <f>IF(P26="O","",P7)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ26" s="1" t="str">
-        <f>IF(Q26="O","",Q7)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM26" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>9</v>
       </c>
@@ -3292,71 +3391,74 @@
         <v>9</v>
       </c>
       <c r="U27" s="1" t="str">
-        <f>IF(B27="O","",B8)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V27" s="1" t="str">
-        <f>IF(C27="O","",C8)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W27" s="1" t="str">
-        <f>IF(D27="O","",D8)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X27" s="1" t="str">
-        <f>IF(E27="O","",E8)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y27" s="1" t="str">
-        <f>IF(F27="O","",F8)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z27" s="1" t="str">
-        <f>IF(G27="O","",G8)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AA27" s="1" t="str">
-        <f>IF(H27="O","",H8)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB27" s="1" t="str">
-        <f>IF(I27="O","",I8)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC27" s="1" t="str">
-        <f>IF(J27="O","",J8)</f>
+        <f t="shared" si="11"/>
         <v>9,8</v>
       </c>
       <c r="AD27" s="1" t="str">
-        <f>IF(K27="O","",K8)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE27" s="1" t="str">
-        <f>IF(L27="O","",L8)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF27" s="1" t="str">
-        <f>IF(M27="O","",M8)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG27" s="1" t="str">
-        <f>IF(N27="O","",N8)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH27" s="1" t="str">
-        <f>IF(O27="O","",O8)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI27" s="1" t="str">
-        <f>IF(P27="O","",P8)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ27" s="1" t="str">
-        <f>IF(Q27="O","",Q8)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM27" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>8</v>
       </c>
@@ -3400,71 +3502,74 @@
         <v>8</v>
       </c>
       <c r="U28" s="1" t="str">
-        <f>IF(B28="O","",B9)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V28" s="1" t="str">
-        <f>IF(C28="O","",C9)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W28" s="1" t="str">
-        <f>IF(D28="O","",D9)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X28" s="1" t="str">
-        <f>IF(E28="O","",E9)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y28" s="1" t="str">
-        <f>IF(F28="O","",F9)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z28" s="1" t="str">
-        <f>IF(G28="O","",G9)</f>
+        <f t="shared" si="8"/>
         <v>8,5</v>
       </c>
       <c r="AA28" s="1" t="str">
-        <f>IF(H28="O","",H9)</f>
+        <f t="shared" si="9"/>
         <v>8,6</v>
       </c>
       <c r="AB28" s="1" t="str">
-        <f>IF(I28="O","",I9)</f>
+        <f t="shared" si="10"/>
         <v>8,7</v>
       </c>
       <c r="AC28" s="1" t="str">
-        <f>IF(J28="O","",J9)</f>
+        <f t="shared" si="11"/>
         <v>8,8</v>
       </c>
       <c r="AD28" s="1" t="str">
-        <f>IF(K28="O","",K9)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE28" s="1" t="str">
-        <f>IF(L28="O","",L9)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF28" s="1" t="str">
-        <f>IF(M28="O","",M9)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG28" s="1" t="str">
-        <f>IF(N28="O","",N9)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH28" s="1" t="str">
-        <f>IF(O28="O","",O9)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI28" s="1" t="str">
-        <f>IF(P28="O","",P9)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ28" s="1" t="str">
-        <f>IF(Q28="O","",Q9)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM28" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>7</v>
       </c>
@@ -3517,71 +3622,74 @@
         <v>7</v>
       </c>
       <c r="U29" s="1" t="str">
-        <f>IF(B29="O","",B10)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V29" s="1" t="str">
-        <f>IF(C29="O","",C10)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W29" s="1" t="str">
-        <f>IF(D29="O","",D10)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X29" s="1" t="str">
-        <f>IF(E29="O","",E10)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y29" s="1" t="str">
-        <f>IF(F29="O","",F10)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z29" s="1" t="str">
-        <f>IF(G29="O","",G10)</f>
+        <f t="shared" si="8"/>
         <v>7,5</v>
       </c>
       <c r="AA29" s="1" t="str">
-        <f>IF(H29="O","",H10)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB29" s="1" t="str">
-        <f>IF(I29="O","",I10)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC29" s="1" t="str">
-        <f>IF(J29="O","",J10)</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AD29" s="1" t="str">
-        <f>IF(K29="O","",K10)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE29" s="1" t="str">
-        <f>IF(L29="O","",L10)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF29" s="1" t="str">
-        <f>IF(M29="O","",M10)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG29" s="1" t="str">
-        <f>IF(N29="O","",N10)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH29" s="1" t="str">
-        <f>IF(O29="O","",O10)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI29" s="1" t="str">
-        <f>IF(P29="O","",P10)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ29" s="1" t="str">
-        <f>IF(Q29="O","",Q10)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM29" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>6</v>
       </c>
@@ -3634,71 +3742,74 @@
         <v>6</v>
       </c>
       <c r="U30" s="1" t="str">
-        <f>IF(B30="O","",B11)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V30" s="1" t="str">
-        <f>IF(C30="O","",C11)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W30" s="1" t="str">
-        <f>IF(D30="O","",D11)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X30" s="1" t="str">
-        <f>IF(E30="O","",E11)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y30" s="1" t="str">
-        <f>IF(F30="O","",F11)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z30" s="1" t="str">
-        <f>IF(G30="O","",G11)</f>
+        <f t="shared" si="8"/>
         <v>6,5</v>
       </c>
       <c r="AA30" s="1" t="str">
-        <f>IF(H30="O","",H11)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB30" s="1" t="str">
-        <f>IF(I30="O","",I11)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC30" s="1" t="str">
-        <f>IF(J30="O","",J11)</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AD30" s="1" t="str">
-        <f>IF(K30="O","",K11)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE30" s="1" t="str">
-        <f>IF(L30="O","",L11)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF30" s="1" t="str">
-        <f>IF(M30="O","",M11)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG30" s="1" t="str">
-        <f>IF(N30="O","",N11)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH30" s="1" t="str">
-        <f>IF(O30="O","",O11)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI30" s="1" t="str">
-        <f>IF(P30="O","",P11)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ30" s="1" t="str">
-        <f>IF(Q30="O","",Q11)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM30" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>5</v>
       </c>
@@ -3751,71 +3862,74 @@
         <v>5</v>
       </c>
       <c r="U31" s="1" t="str">
-        <f>IF(B31="O","",B12)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V31" s="1" t="str">
-        <f>IF(C31="O","",C12)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W31" s="1" t="str">
-        <f>IF(D31="O","",D12)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X31" s="1" t="str">
-        <f>IF(E31="O","",E12)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y31" s="1" t="str">
-        <f>IF(F31="O","",F12)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z31" s="1" t="str">
-        <f>IF(G31="O","",G12)</f>
+        <f t="shared" si="8"/>
         <v>5,5</v>
       </c>
       <c r="AA31" s="1" t="str">
-        <f>IF(H31="O","",H12)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB31" s="1" t="str">
-        <f>IF(I31="O","",I12)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC31" s="1" t="str">
-        <f>IF(J31="O","",J12)</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AD31" s="1" t="str">
-        <f>IF(K31="O","",K12)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE31" s="1" t="str">
-        <f>IF(L31="O","",L12)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF31" s="1" t="str">
-        <f>IF(M31="O","",M12)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG31" s="1" t="str">
-        <f>IF(N31="O","",N12)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH31" s="1" t="str">
-        <f>IF(O31="O","",O12)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI31" s="1" t="str">
-        <f>IF(P31="O","",P12)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ31" s="1" t="str">
-        <f>IF(Q31="O","",Q12)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM31" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -3868,71 +3982,74 @@
         <v>4</v>
       </c>
       <c r="U32" s="1" t="str">
-        <f>IF(B32="O","",B13)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V32" s="1" t="str">
-        <f>IF(C32="O","",C13)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W32" s="1" t="str">
-        <f>IF(D32="O","",D13)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X32" s="1" t="str">
-        <f>IF(E32="O","",E13)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y32" s="1" t="str">
-        <f>IF(F32="O","",F13)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z32" s="1" t="str">
-        <f>IF(G32="O","",G13)</f>
+        <f t="shared" si="8"/>
         <v>4,5</v>
       </c>
       <c r="AA32" s="1" t="str">
-        <f>IF(H32="O","",H13)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB32" s="1" t="str">
-        <f>IF(I32="O","",I13)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC32" s="1" t="str">
-        <f>IF(J32="O","",J13)</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AD32" s="1" t="str">
-        <f>IF(K32="O","",K13)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE32" s="1" t="str">
-        <f>IF(L32="O","",L13)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF32" s="1" t="str">
-        <f>IF(M32="O","",M13)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG32" s="1" t="str">
-        <f>IF(N32="O","",N13)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH32" s="1" t="str">
-        <f>IF(O32="O","",O13)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI32" s="1" t="str">
-        <f>IF(P32="O","",P13)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ32" s="1" t="str">
-        <f>IF(Q32="O","",Q13)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM32" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -3985,71 +4102,74 @@
         <v>3</v>
       </c>
       <c r="U33" s="1" t="str">
-        <f>IF(B33="O","",B14)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V33" s="1" t="str">
-        <f>IF(C33="O","",C14)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W33" s="1" t="str">
-        <f>IF(D33="O","",D14)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X33" s="1" t="str">
-        <f>IF(E33="O","",E14)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y33" s="1" t="str">
-        <f>IF(F33="O","",F14)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z33" s="1" t="str">
-        <f>IF(G33="O","",G14)</f>
+        <f t="shared" si="8"/>
         <v>3,5</v>
       </c>
       <c r="AA33" s="1" t="str">
-        <f>IF(H33="O","",H14)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB33" s="1" t="str">
-        <f>IF(I33="O","",I14)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC33" s="1" t="str">
-        <f>IF(J33="O","",J14)</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AD33" s="1" t="str">
-        <f>IF(K33="O","",K14)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE33" s="1" t="str">
-        <f>IF(L33="O","",L14)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF33" s="1" t="str">
-        <f>IF(M33="O","",M14)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG33" s="1" t="str">
-        <f>IF(N33="O","",N14)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH33" s="1" t="str">
-        <f>IF(O33="O","",O14)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI33" s="1" t="str">
-        <f>IF(P33="O","",P14)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ33" s="1" t="str">
-        <f>IF(Q33="O","",Q14)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM33" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2</v>
       </c>
@@ -4102,71 +4222,74 @@
         <v>2</v>
       </c>
       <c r="U34" s="1" t="str">
-        <f>IF(B34="O","",B15)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V34" s="1" t="str">
-        <f>IF(C34="O","",C15)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W34" s="1" t="str">
-        <f>IF(D34="O","",D15)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X34" s="1" t="str">
-        <f>IF(E34="O","",E15)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y34" s="1" t="str">
-        <f>IF(F34="O","",F15)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z34" s="1" t="str">
-        <f>IF(G34="O","",G15)</f>
+        <f t="shared" si="8"/>
         <v>2,5</v>
       </c>
       <c r="AA34" s="1" t="str">
-        <f>IF(H34="O","",H15)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB34" s="1" t="str">
-        <f>IF(I34="O","",I15)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC34" s="1" t="str">
-        <f>IF(J34="O","",J15)</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AD34" s="1" t="str">
-        <f>IF(K34="O","",K15)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE34" s="1" t="str">
-        <f>IF(L34="O","",L15)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF34" s="1" t="str">
-        <f>IF(M34="O","",M15)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG34" s="1" t="str">
-        <f>IF(N34="O","",N15)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH34" s="1" t="str">
-        <f>IF(O34="O","",O15)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI34" s="1" t="str">
-        <f>IF(P34="O","",P15)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ34" s="1" t="str">
-        <f>IF(Q34="O","",Q15)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM34" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -4219,71 +4342,74 @@
         <v>1</v>
       </c>
       <c r="U35" s="1" t="str">
-        <f>IF(B35="O","",B16)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V35" s="1" t="str">
-        <f>IF(C35="O","",C16)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W35" s="1" t="str">
-        <f>IF(D35="O","",D16)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X35" s="1" t="str">
-        <f>IF(E35="O","",E16)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y35" s="1" t="str">
-        <f>IF(F35="O","",F16)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z35" s="1" t="str">
-        <f>IF(G35="O","",G16)</f>
+        <f t="shared" si="8"/>
         <v>1,5</v>
       </c>
       <c r="AA35" s="1" t="str">
-        <f>IF(H35="O","",H16)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB35" s="1" t="str">
-        <f>IF(I35="O","",I16)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC35" s="1" t="str">
-        <f>IF(J35="O","",J16)</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AD35" s="1" t="str">
-        <f>IF(K35="O","",K16)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE35" s="1" t="str">
-        <f>IF(L35="O","",L16)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF35" s="1" t="str">
-        <f>IF(M35="O","",M16)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG35" s="1" t="str">
-        <f>IF(N35="O","",N16)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH35" s="1" t="str">
-        <f>IF(O35="O","",O16)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI35" s="1" t="str">
-        <f>IF(P35="O","",P16)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ35" s="1" t="str">
-        <f>IF(Q35="O","",Q16)</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AM35" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>0</v>
       </c>
@@ -4330,68 +4456,96 @@
         <v>0</v>
       </c>
       <c r="U36" s="1" t="str">
-        <f>IF(B36="O","",B17)</f>
+        <f t="shared" si="3"/>
         <v>0,0</v>
       </c>
       <c r="V36" s="1" t="str">
-        <f>IF(C36="O","",C17)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W36" s="1" t="str">
-        <f>IF(D36="O","",D17)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X36" s="1" t="str">
-        <f>IF(E36="O","",E17)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y36" s="1" t="str">
-        <f>IF(F36="O","",F17)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z36" s="1" t="str">
-        <f>IF(G36="O","",G17)</f>
+        <f t="shared" si="8"/>
         <v>0,5</v>
       </c>
       <c r="AA36" s="1" t="str">
-        <f>IF(H36="O","",H17)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB36" s="1" t="str">
-        <f>IF(I36="O","",I17)</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AC36" s="1" t="str">
-        <f>IF(J36="O","",J17)</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AD36" s="1" t="str">
-        <f>IF(K36="O","",K17)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE36" s="1" t="str">
-        <f>IF(L36="O","",L17)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AF36" s="1" t="str">
-        <f>IF(M36="O","",M17)</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AG36" s="1" t="str">
-        <f>IF(N36="O","",N17)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH36" s="1" t="str">
-        <f>IF(O36="O","",O17)</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AI36" s="1" t="str">
-        <f>IF(P36="O","",P17)</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AJ36" s="1" t="str">
-        <f>IF(Q36="O","",Q17)</f>
+        <f t="shared" si="18"/>
         <v>0,15</v>
+      </c>
+      <c r="AM36" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM37" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM38" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM39" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM40" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM41" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementando colisiones 2 (Solo hay un pequeño bug)
</commit_message>
<xml_diff>
--- a/mapfiles/template_maps.xlsx
+++ b/mapfiles/template_maps.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,12 +10,12 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="26">
   <si>
     <t>map1</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>0,10</t>
+  </si>
+  <si>
+    <t>test collisions</t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,7 +230,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM41"/>
+  <dimension ref="A1:AM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL11" sqref="AL11"/>
+    <sheetView tabSelected="1" topLeftCell="L34" workbookViewId="0">
+      <selection activeCell="AB55" sqref="AB55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2637,67 +2640,67 @@
         <v>15</v>
       </c>
       <c r="U21" s="1" t="str">
-        <f t="shared" ref="U21:U36" si="3">IF(B21="O","",B2)</f>
+        <f>IF(B42="O","",B2)</f>
         <v>15,15</v>
       </c>
       <c r="V21" s="1" t="str">
-        <f t="shared" ref="V21:V36" si="4">IF(C21="O","",C2)</f>
+        <f t="shared" ref="V21:V36" si="3">IF(C21="O","",C2)</f>
         <v/>
       </c>
       <c r="W21" s="1" t="str">
-        <f t="shared" ref="W21:W36" si="5">IF(D21="O","",D2)</f>
+        <f t="shared" ref="W21:W36" si="4">IF(D21="O","",D2)</f>
         <v/>
       </c>
       <c r="X21" s="1" t="str">
-        <f t="shared" ref="X21:X36" si="6">IF(E21="O","",E2)</f>
+        <f t="shared" ref="X21:X36" si="5">IF(E21="O","",E2)</f>
         <v/>
       </c>
       <c r="Y21" s="1" t="str">
-        <f t="shared" ref="Y21:Y36" si="7">IF(F21="O","",F2)</f>
+        <f t="shared" ref="Y21:Y36" si="6">IF(F21="O","",F2)</f>
         <v/>
       </c>
       <c r="Z21" s="1" t="str">
-        <f t="shared" ref="Z21:Z27" si="8">IF(G21="O","",G2)</f>
+        <f t="shared" ref="Z21:Z27" si="7">IF(G21="O","",G2)</f>
         <v/>
       </c>
       <c r="AA21" s="1" t="str">
-        <f t="shared" ref="AA21:AA36" si="9">IF(H21="O","",H2)</f>
+        <f t="shared" ref="AA21:AA36" si="8">IF(H21="O","",H2)</f>
         <v/>
       </c>
       <c r="AB21" s="1" t="str">
-        <f t="shared" ref="AB21:AB36" si="10">IF(I21="O","",I2)</f>
+        <f t="shared" ref="AB21:AB36" si="9">IF(I21="O","",I2)</f>
         <v/>
       </c>
       <c r="AC21" s="1" t="str">
-        <f t="shared" ref="AC21:AC36" si="11">IF(J21="O","",J2)</f>
+        <f t="shared" ref="AC21:AC36" si="10">IF(J21="O","",J2)</f>
         <v>15,7</v>
       </c>
       <c r="AD21" s="1" t="str">
-        <f t="shared" ref="AD21:AD36" si="12">IF(K21="O","",K2)</f>
+        <f t="shared" ref="AD21:AD36" si="11">IF(K21="O","",K2)</f>
         <v/>
       </c>
       <c r="AE21" s="1" t="str">
-        <f t="shared" ref="AE21:AE36" si="13">IF(L21="O","",L2)</f>
+        <f t="shared" ref="AE21:AE36" si="12">IF(L21="O","",L2)</f>
         <v/>
       </c>
       <c r="AF21" s="1" t="str">
-        <f t="shared" ref="AF21:AF36" si="14">IF(M21="O","",M2)</f>
+        <f t="shared" ref="AF21:AF36" si="13">IF(M21="O","",M2)</f>
         <v/>
       </c>
       <c r="AG21" s="1" t="str">
-        <f t="shared" ref="AG21:AG36" si="15">IF(N21="O","",N2)</f>
+        <f t="shared" ref="AG21:AG36" si="14">IF(N21="O","",N2)</f>
         <v/>
       </c>
       <c r="AH21" s="1" t="str">
-        <f t="shared" ref="AH21:AH36" si="16">IF(O21="O","",O2)</f>
+        <f t="shared" ref="AH21:AH36" si="15">IF(O21="O","",O2)</f>
         <v/>
       </c>
       <c r="AI21" s="1" t="str">
-        <f t="shared" ref="AI21:AI36" si="17">IF(P21="O","",P2)</f>
+        <f t="shared" ref="AI21:AI36" si="16">IF(P21="O","",P2)</f>
         <v/>
       </c>
       <c r="AJ21" s="1" t="str">
-        <f t="shared" ref="AJ21:AJ36" si="18">IF(Q21="O","",Q2)</f>
+        <f t="shared" ref="AJ21:AJ36" si="17">IF(Q21="O","",Q2)</f>
         <v/>
       </c>
       <c r="AM21" s="2" t="s">
@@ -2757,67 +2760,67 @@
         <v>14</v>
       </c>
       <c r="U22" s="1" t="str">
+        <f t="shared" ref="U21:U36" si="18">IF(B22="O","",B3)</f>
+        <v/>
+      </c>
+      <c r="V22" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V22" s="1" t="str">
+      <c r="W22" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W22" s="1" t="str">
+      <c r="X22" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X22" s="1" t="str">
+      <c r="Y22" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y22" s="1" t="str">
+      <c r="Z22" s="1" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="Z22" s="1" t="str">
+      <c r="AA22" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AA22" s="1" t="str">
+      <c r="AB22" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB22" s="1" t="str">
+      <c r="AC22" s="1" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AC22" s="1" t="str">
+        <v>14,7</v>
+      </c>
+      <c r="AD22" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>14,7</v>
-      </c>
-      <c r="AD22" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AE22" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE22" s="1" t="str">
+      <c r="AF22" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF22" s="1" t="str">
+      <c r="AG22" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG22" s="1" t="str">
+      <c r="AH22" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH22" s="1" t="str">
+      <c r="AI22" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI22" s="1" t="str">
+      <c r="AJ22" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ22" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM22" s="2" t="s">
@@ -2877,67 +2880,67 @@
         <v>13</v>
       </c>
       <c r="U23" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V23" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V23" s="1" t="str">
+      <c r="W23" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W23" s="1" t="str">
+      <c r="X23" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X23" s="1" t="str">
+      <c r="Y23" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y23" s="1" t="str">
+      <c r="Z23" s="1" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="Z23" s="1" t="str">
+      <c r="AA23" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AA23" s="1" t="str">
+      <c r="AB23" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB23" s="1" t="str">
+      <c r="AC23" s="1" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AC23" s="1" t="str">
+        <v>13,7</v>
+      </c>
+      <c r="AD23" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>13,7</v>
-      </c>
-      <c r="AD23" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AE23" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE23" s="1" t="str">
+      <c r="AF23" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF23" s="1" t="str">
+      <c r="AG23" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG23" s="1" t="str">
+      <c r="AH23" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH23" s="1" t="str">
+      <c r="AI23" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI23" s="1" t="str">
+      <c r="AJ23" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ23" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM23" s="2" t="s">
@@ -2997,67 +3000,67 @@
         <v>12</v>
       </c>
       <c r="U24" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V24" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V24" s="1" t="str">
+      <c r="W24" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W24" s="1" t="str">
+      <c r="X24" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X24" s="1" t="str">
+      <c r="Y24" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y24" s="1" t="str">
+      <c r="Z24" s="1" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="Z24" s="1" t="str">
+      <c r="AA24" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AA24" s="1" t="str">
+      <c r="AB24" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB24" s="1" t="str">
+      <c r="AC24" s="1" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AC24" s="1" t="str">
+        <v>12,7</v>
+      </c>
+      <c r="AD24" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>12,7</v>
-      </c>
-      <c r="AD24" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AE24" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE24" s="1" t="str">
+      <c r="AF24" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF24" s="1" t="str">
+      <c r="AG24" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG24" s="1" t="str">
+      <c r="AH24" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH24" s="1" t="str">
+      <c r="AI24" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI24" s="1" t="str">
+      <c r="AJ24" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ24" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM24" s="2" t="s">
@@ -3117,67 +3120,67 @@
         <v>11</v>
       </c>
       <c r="U25" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V25" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V25" s="1" t="str">
+      <c r="W25" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W25" s="1" t="str">
+      <c r="X25" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X25" s="1" t="str">
+      <c r="Y25" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y25" s="1" t="str">
+      <c r="Z25" s="1" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="Z25" s="1" t="str">
+      <c r="AA25" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AA25" s="1" t="str">
+      <c r="AB25" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB25" s="1" t="str">
+      <c r="AC25" s="1" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AC25" s="1" t="str">
+        <v>11,7</v>
+      </c>
+      <c r="AD25" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>11,7</v>
-      </c>
-      <c r="AD25" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AE25" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE25" s="1" t="str">
+      <c r="AF25" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF25" s="1" t="str">
+      <c r="AG25" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG25" s="1" t="str">
+      <c r="AH25" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH25" s="1" t="str">
+      <c r="AI25" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI25" s="1" t="str">
+      <c r="AJ25" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ25" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM25" s="2" t="s">
@@ -3237,67 +3240,67 @@
         <v>10</v>
       </c>
       <c r="U26" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V26" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V26" s="1" t="str">
+      <c r="W26" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W26" s="1" t="str">
+      <c r="X26" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X26" s="1" t="str">
+      <c r="Y26" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y26" s="1" t="str">
+      <c r="Z26" s="1" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="Z26" s="1" t="str">
+      <c r="AA26" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AA26" s="1" t="str">
+      <c r="AB26" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB26" s="1" t="str">
+      <c r="AC26" s="1" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AC26" s="1" t="str">
+        <v>10,7</v>
+      </c>
+      <c r="AD26" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>10,7</v>
-      </c>
-      <c r="AD26" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AE26" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE26" s="1" t="str">
+      <c r="AF26" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF26" s="1" t="str">
+      <c r="AG26" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG26" s="1" t="str">
+      <c r="AH26" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH26" s="1" t="str">
+      <c r="AI26" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI26" s="1" t="str">
+      <c r="AJ26" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ26" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM26" s="2" t="s">
@@ -3357,67 +3360,67 @@
         <v>9</v>
       </c>
       <c r="U27" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V27" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V27" s="1" t="str">
+      <c r="W27" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W27" s="1" t="str">
+      <c r="X27" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X27" s="1" t="str">
+      <c r="Y27" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y27" s="1" t="str">
+      <c r="Z27" s="1" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="Z27" s="1" t="str">
+      <c r="AA27" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AA27" s="1" t="str">
+      <c r="AB27" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB27" s="1" t="str">
+      <c r="AC27" s="1" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AC27" s="1" t="str">
+        <v>9,7</v>
+      </c>
+      <c r="AD27" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>9,7</v>
-      </c>
-      <c r="AD27" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AE27" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE27" s="1" t="str">
+      <c r="AF27" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF27" s="1" t="str">
+      <c r="AG27" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG27" s="1" t="str">
+      <c r="AH27" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH27" s="1" t="str">
+      <c r="AI27" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI27" s="1" t="str">
+      <c r="AJ27" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ27" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM27" s="2" t="s">
@@ -3468,67 +3471,67 @@
         <v>8</v>
       </c>
       <c r="U28" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V28" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V28" s="1" t="str">
+      <c r="W28" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W28" s="1" t="str">
+      <c r="X28" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X28" s="1" t="str">
+      <c r="Y28" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y28" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
       <c r="Z28" s="1" t="str">
-        <f>IF(G28="O","",G9)</f>
+        <f t="shared" ref="Z28:Z36" si="19">IF(G28="O","",G9)</f>
         <v>8,10</v>
       </c>
       <c r="AA28" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>8,9</v>
+      </c>
+      <c r="AB28" s="1" t="str">
         <f t="shared" si="9"/>
-        <v>8,9</v>
-      </c>
-      <c r="AB28" s="1" t="str">
+        <v>8,8</v>
+      </c>
+      <c r="AC28" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>8,8</v>
-      </c>
-      <c r="AC28" s="1" t="str">
+        <v>8,7</v>
+      </c>
+      <c r="AD28" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>8,7</v>
-      </c>
-      <c r="AD28" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AE28" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE28" s="1" t="str">
+      <c r="AF28" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF28" s="1" t="str">
+      <c r="AG28" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG28" s="1" t="str">
+      <c r="AH28" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH28" s="1" t="str">
+      <c r="AI28" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI28" s="1" t="str">
+      <c r="AJ28" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ28" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM28" s="2" t="s">
@@ -3588,67 +3591,67 @@
         <v>7</v>
       </c>
       <c r="U29" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V29" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V29" s="1" t="str">
+      <c r="W29" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W29" s="1" t="str">
+      <c r="X29" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X29" s="1" t="str">
+      <c r="Y29" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y29" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
       <c r="Z29" s="1" t="str">
-        <f>IF(G29="O","",G10)</f>
+        <f t="shared" si="19"/>
         <v>7,10</v>
       </c>
       <c r="AA29" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB29" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB29" s="1" t="str">
+      <c r="AC29" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AC29" s="1" t="str">
+      <c r="AD29" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AD29" s="1" t="str">
+      <c r="AE29" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE29" s="1" t="str">
+      <c r="AF29" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF29" s="1" t="str">
+      <c r="AG29" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG29" s="1" t="str">
+      <c r="AH29" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH29" s="1" t="str">
+      <c r="AI29" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI29" s="1" t="str">
+      <c r="AJ29" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ29" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM29" s="2" t="s">
@@ -3708,67 +3711,67 @@
         <v>6</v>
       </c>
       <c r="U30" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V30" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V30" s="1" t="str">
+      <c r="W30" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W30" s="1" t="str">
+      <c r="X30" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X30" s="1" t="str">
+      <c r="Y30" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y30" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
       <c r="Z30" s="1" t="str">
-        <f>IF(G30="O","",G11)</f>
+        <f t="shared" si="19"/>
         <v>6,10</v>
       </c>
       <c r="AA30" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB30" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB30" s="1" t="str">
+      <c r="AC30" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AC30" s="1" t="str">
+      <c r="AD30" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AD30" s="1" t="str">
+      <c r="AE30" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE30" s="1" t="str">
+      <c r="AF30" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF30" s="1" t="str">
+      <c r="AG30" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG30" s="1" t="str">
+      <c r="AH30" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH30" s="1" t="str">
+      <c r="AI30" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI30" s="1" t="str">
+      <c r="AJ30" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ30" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM30" s="2" t="s">
@@ -3828,67 +3831,67 @@
         <v>5</v>
       </c>
       <c r="U31" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V31" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V31" s="1" t="str">
+      <c r="W31" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W31" s="1" t="str">
+      <c r="X31" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X31" s="1" t="str">
+      <c r="Y31" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y31" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
       <c r="Z31" s="1" t="str">
-        <f>IF(G31="O","",G12)</f>
+        <f t="shared" si="19"/>
         <v>5,10</v>
       </c>
       <c r="AA31" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB31" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB31" s="1" t="str">
+      <c r="AC31" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AC31" s="1" t="str">
+      <c r="AD31" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AD31" s="1" t="str">
+      <c r="AE31" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE31" s="1" t="str">
+      <c r="AF31" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF31" s="1" t="str">
+      <c r="AG31" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG31" s="1" t="str">
+      <c r="AH31" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH31" s="1" t="str">
+      <c r="AI31" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI31" s="1" t="str">
+      <c r="AJ31" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ31" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM31" s="1" t="s">
@@ -3948,67 +3951,67 @@
         <v>4</v>
       </c>
       <c r="U32" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V32" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V32" s="1" t="str">
+      <c r="W32" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W32" s="1" t="str">
+      <c r="X32" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X32" s="1" t="str">
+      <c r="Y32" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y32" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
       <c r="Z32" s="1" t="str">
-        <f>IF(G32="O","",G13)</f>
+        <f t="shared" si="19"/>
         <v>4,10</v>
       </c>
       <c r="AA32" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB32" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB32" s="1" t="str">
+      <c r="AC32" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AC32" s="1" t="str">
+      <c r="AD32" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AD32" s="1" t="str">
+      <c r="AE32" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE32" s="1" t="str">
+      <c r="AF32" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF32" s="1" t="str">
+      <c r="AG32" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG32" s="1" t="str">
+      <c r="AH32" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH32" s="1" t="str">
+      <c r="AI32" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI32" s="1" t="str">
+      <c r="AJ32" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ32" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM32" s="1" t="s">
@@ -4068,67 +4071,67 @@
         <v>3</v>
       </c>
       <c r="U33" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V33" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V33" s="1" t="str">
+      <c r="W33" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W33" s="1" t="str">
+      <c r="X33" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X33" s="1" t="str">
+      <c r="Y33" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y33" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
       <c r="Z33" s="1" t="str">
-        <f>IF(G33="O","",G14)</f>
+        <f t="shared" si="19"/>
         <v>3,10</v>
       </c>
       <c r="AA33" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB33" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB33" s="1" t="str">
+      <c r="AC33" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AC33" s="1" t="str">
+      <c r="AD33" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AD33" s="1" t="str">
+      <c r="AE33" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE33" s="1" t="str">
+      <c r="AF33" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF33" s="1" t="str">
+      <c r="AG33" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG33" s="1" t="str">
+      <c r="AH33" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH33" s="1" t="str">
+      <c r="AI33" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI33" s="1" t="str">
+      <c r="AJ33" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ33" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM33" s="1" t="s">
@@ -4188,67 +4191,67 @@
         <v>2</v>
       </c>
       <c r="U34" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V34" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V34" s="1" t="str">
+      <c r="W34" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W34" s="1" t="str">
+      <c r="X34" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X34" s="1" t="str">
+      <c r="Y34" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y34" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
       <c r="Z34" s="1" t="str">
-        <f>IF(G34="O","",G15)</f>
+        <f t="shared" si="19"/>
         <v>2,10</v>
       </c>
       <c r="AA34" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB34" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB34" s="1" t="str">
+      <c r="AC34" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AC34" s="1" t="str">
+      <c r="AD34" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AD34" s="1" t="str">
+      <c r="AE34" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE34" s="1" t="str">
+      <c r="AF34" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF34" s="1" t="str">
+      <c r="AG34" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG34" s="1" t="str">
+      <c r="AH34" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH34" s="1" t="str">
+      <c r="AI34" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI34" s="1" t="str">
+      <c r="AJ34" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ34" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM34" s="1" t="s">
@@ -4308,67 +4311,67 @@
         <v>1</v>
       </c>
       <c r="U35" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="V35" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V35" s="1" t="str">
+      <c r="W35" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W35" s="1" t="str">
+      <c r="X35" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X35" s="1" t="str">
+      <c r="Y35" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y35" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
       <c r="Z35" s="1" t="str">
-        <f>IF(G35="O","",G16)</f>
+        <f t="shared" si="19"/>
         <v>1,10</v>
       </c>
       <c r="AA35" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB35" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB35" s="1" t="str">
+      <c r="AC35" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AC35" s="1" t="str">
+      <c r="AD35" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AD35" s="1" t="str">
+      <c r="AE35" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE35" s="1" t="str">
+      <c r="AF35" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF35" s="1" t="str">
+      <c r="AG35" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG35" s="1" t="str">
+      <c r="AH35" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH35" s="1" t="str">
+      <c r="AI35" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI35" s="1" t="str">
+      <c r="AJ35" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ35" s="1" t="str">
-        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AM35" s="1" t="s">
@@ -4422,67 +4425,67 @@
         <v>0</v>
       </c>
       <c r="U36" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0,15</v>
+      </c>
+      <c r="V36" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0,15</v>
-      </c>
-      <c r="V36" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W36" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W36" s="1" t="str">
+      <c r="X36" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X36" s="1" t="str">
+      <c r="Y36" s="1" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Y36" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
       <c r="Z36" s="1" t="str">
-        <f>IF(G36="O","",G17)</f>
+        <f t="shared" si="19"/>
         <v>0,10</v>
       </c>
       <c r="AA36" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AB36" s="1" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB36" s="1" t="str">
+      <c r="AC36" s="1" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AC36" s="1" t="str">
+      <c r="AD36" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AD36" s="1" t="str">
+      <c r="AE36" s="1" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AE36" s="1" t="str">
+      <c r="AF36" s="1" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AF36" s="1" t="str">
+      <c r="AG36" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AG36" s="1" t="str">
+      <c r="AH36" s="1" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="AH36" s="1" t="str">
+      <c r="AI36" s="1" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AI36" s="1" t="str">
+      <c r="AJ36" s="1" t="str">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AJ36" s="1" t="str">
-        <f t="shared" si="18"/>
         <v>0,0</v>
       </c>
       <c r="AM36" s="1" t="s">
@@ -4505,13 +4508,1267 @@
       </c>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="AM40" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>15</v>
+      </c>
+      <c r="C41" s="1">
+        <v>14</v>
+      </c>
+      <c r="D41" s="1">
+        <v>13</v>
+      </c>
+      <c r="E41" s="1">
+        <v>12</v>
+      </c>
+      <c r="F41" s="1">
+        <v>11</v>
+      </c>
+      <c r="G41" s="1">
+        <v>10</v>
+      </c>
+      <c r="H41" s="1">
+        <v>9</v>
+      </c>
+      <c r="I41" s="1">
+        <v>8</v>
+      </c>
+      <c r="J41" s="1">
+        <v>7</v>
+      </c>
+      <c r="K41" s="1">
+        <v>6</v>
+      </c>
+      <c r="L41" s="1">
+        <v>5</v>
+      </c>
+      <c r="M41" s="1">
+        <v>4</v>
+      </c>
+      <c r="N41" s="1">
+        <v>3</v>
+      </c>
+      <c r="O41" s="1">
+        <v>2</v>
+      </c>
+      <c r="P41" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>0</v>
+      </c>
+      <c r="U41" s="1">
+        <v>15</v>
+      </c>
+      <c r="V41" s="1">
+        <v>14</v>
+      </c>
+      <c r="W41" s="1">
+        <v>13</v>
+      </c>
+      <c r="X41" s="1">
+        <v>12</v>
+      </c>
+      <c r="Y41" s="1">
+        <v>11</v>
+      </c>
+      <c r="Z41" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA41" s="1">
+        <v>9</v>
+      </c>
+      <c r="AB41" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC41" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD41" s="1">
+        <v>6</v>
+      </c>
+      <c r="AE41" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF41" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG41" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH41" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ41" s="1">
+        <v>0</v>
+      </c>
       <c r="AM41" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>15</v>
+      </c>
+      <c r="T42" s="1">
+        <v>15</v>
+      </c>
+      <c r="U42" s="1" t="str">
+        <f>IF(B42="O","",B2)</f>
+        <v>15,15</v>
+      </c>
+      <c r="V42" s="1" t="str">
+        <f t="shared" ref="V42:AJ42" si="20">IF(C42="O","",C2)</f>
+        <v>15,14</v>
+      </c>
+      <c r="W42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,13</v>
+      </c>
+      <c r="X42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,12</v>
+      </c>
+      <c r="Y42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,11</v>
+      </c>
+      <c r="Z42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,10</v>
+      </c>
+      <c r="AA42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,9</v>
+      </c>
+      <c r="AB42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,8</v>
+      </c>
+      <c r="AC42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,7</v>
+      </c>
+      <c r="AD42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,6</v>
+      </c>
+      <c r="AE42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,5</v>
+      </c>
+      <c r="AF42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,4</v>
+      </c>
+      <c r="AG42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,3</v>
+      </c>
+      <c r="AH42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,2</v>
+      </c>
+      <c r="AI42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,1</v>
+      </c>
+      <c r="AJ42" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>15,0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>14</v>
+      </c>
+      <c r="T43" s="1">
+        <v>14</v>
+      </c>
+      <c r="U43" s="1" t="str">
+        <f t="shared" ref="U43:U57" si="21">IF(B43="O","",B3)</f>
+        <v>14,15</v>
+      </c>
+      <c r="V43" s="1" t="str">
+        <f t="shared" ref="V43:V57" si="22">IF(C43="O","",C3)</f>
+        <v>14,14</v>
+      </c>
+      <c r="W43" s="1" t="str">
+        <f t="shared" ref="W43:W57" si="23">IF(D43="O","",D3)</f>
+        <v>14,13</v>
+      </c>
+      <c r="X43" s="1" t="str">
+        <f t="shared" ref="X43:X57" si="24">IF(E43="O","",E3)</f>
+        <v>14,12</v>
+      </c>
+      <c r="Y43" s="1" t="str">
+        <f t="shared" ref="Y43:Y57" si="25">IF(F43="O","",F3)</f>
+        <v>14,11</v>
+      </c>
+      <c r="Z43" s="1" t="str">
+        <f t="shared" ref="Z43:Z57" si="26">IF(G43="O","",G3)</f>
+        <v>14,10</v>
+      </c>
+      <c r="AA43" s="1" t="str">
+        <f t="shared" ref="AA43:AA57" si="27">IF(H43="O","",H3)</f>
+        <v>14,9</v>
+      </c>
+      <c r="AB43" s="1" t="str">
+        <f t="shared" ref="AB43:AB57" si="28">IF(I43="O","",I3)</f>
+        <v>14,8</v>
+      </c>
+      <c r="AC43" s="1" t="str">
+        <f t="shared" ref="AC43:AC57" si="29">IF(J43="O","",J3)</f>
+        <v>14,7</v>
+      </c>
+      <c r="AD43" s="1" t="str">
+        <f t="shared" ref="AD43:AD57" si="30">IF(K43="O","",K3)</f>
+        <v>14,6</v>
+      </c>
+      <c r="AE43" s="1" t="str">
+        <f t="shared" ref="AE43:AE57" si="31">IF(L43="O","",L3)</f>
+        <v>14,5</v>
+      </c>
+      <c r="AF43" s="1" t="str">
+        <f t="shared" ref="AF43:AF57" si="32">IF(M43="O","",M3)</f>
+        <v>14,4</v>
+      </c>
+      <c r="AG43" s="1" t="str">
+        <f t="shared" ref="AG43:AG57" si="33">IF(N43="O","",N3)</f>
+        <v>14,3</v>
+      </c>
+      <c r="AH43" s="1" t="str">
+        <f t="shared" ref="AH43:AH57" si="34">IF(O43="O","",O3)</f>
+        <v>14,2</v>
+      </c>
+      <c r="AI43" s="1" t="str">
+        <f t="shared" ref="AI43:AI57" si="35">IF(P43="O","",P3)</f>
+        <v>14,1</v>
+      </c>
+      <c r="AJ43" s="1" t="str">
+        <f t="shared" ref="AJ43:AJ57" si="36">IF(Q43="O","",Q3)</f>
+        <v>14,0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>13</v>
+      </c>
+      <c r="T44" s="1">
+        <v>13</v>
+      </c>
+      <c r="U44" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>13,15</v>
+      </c>
+      <c r="V44" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>13,14</v>
+      </c>
+      <c r="W44" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>13,13</v>
+      </c>
+      <c r="X44" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>13,12</v>
+      </c>
+      <c r="Y44" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>13,11</v>
+      </c>
+      <c r="Z44" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>13,10</v>
+      </c>
+      <c r="AA44" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>13,9</v>
+      </c>
+      <c r="AB44" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>13,8</v>
+      </c>
+      <c r="AC44" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>13,7</v>
+      </c>
+      <c r="AD44" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>13,6</v>
+      </c>
+      <c r="AE44" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>13,5</v>
+      </c>
+      <c r="AF44" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>13,4</v>
+      </c>
+      <c r="AG44" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>13,3</v>
+      </c>
+      <c r="AH44" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>13,2</v>
+      </c>
+      <c r="AI44" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>13,1</v>
+      </c>
+      <c r="AJ44" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>13,0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>12</v>
+      </c>
+      <c r="T45" s="1">
+        <v>12</v>
+      </c>
+      <c r="U45" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>12,15</v>
+      </c>
+      <c r="V45" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>12,14</v>
+      </c>
+      <c r="W45" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>12,13</v>
+      </c>
+      <c r="X45" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>12,12</v>
+      </c>
+      <c r="Y45" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>12,11</v>
+      </c>
+      <c r="Z45" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>12,10</v>
+      </c>
+      <c r="AA45" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>12,9</v>
+      </c>
+      <c r="AB45" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>12,8</v>
+      </c>
+      <c r="AC45" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>12,7</v>
+      </c>
+      <c r="AD45" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>12,6</v>
+      </c>
+      <c r="AE45" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>12,5</v>
+      </c>
+      <c r="AF45" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>12,4</v>
+      </c>
+      <c r="AG45" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>12,3</v>
+      </c>
+      <c r="AH45" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>12,2</v>
+      </c>
+      <c r="AI45" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>12,1</v>
+      </c>
+      <c r="AJ45" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>12,0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>11</v>
+      </c>
+      <c r="T46" s="1">
+        <v>11</v>
+      </c>
+      <c r="U46" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>11,15</v>
+      </c>
+      <c r="V46" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>11,14</v>
+      </c>
+      <c r="W46" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>11,13</v>
+      </c>
+      <c r="X46" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>11,12</v>
+      </c>
+      <c r="Y46" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>11,11</v>
+      </c>
+      <c r="Z46" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>11,10</v>
+      </c>
+      <c r="AA46" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>11,9</v>
+      </c>
+      <c r="AB46" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>11,8</v>
+      </c>
+      <c r="AC46" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>11,7</v>
+      </c>
+      <c r="AD46" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>11,6</v>
+      </c>
+      <c r="AE46" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>11,5</v>
+      </c>
+      <c r="AF46" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>11,4</v>
+      </c>
+      <c r="AG46" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>11,3</v>
+      </c>
+      <c r="AH46" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>11,2</v>
+      </c>
+      <c r="AI46" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>11,1</v>
+      </c>
+      <c r="AJ46" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>11,0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>10</v>
+      </c>
+      <c r="T47" s="1">
+        <v>10</v>
+      </c>
+      <c r="U47" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>10,15</v>
+      </c>
+      <c r="V47" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>10,14</v>
+      </c>
+      <c r="W47" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>10,13</v>
+      </c>
+      <c r="X47" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>10,12</v>
+      </c>
+      <c r="Y47" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>10,11</v>
+      </c>
+      <c r="Z47" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>10,10</v>
+      </c>
+      <c r="AA47" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>10,9</v>
+      </c>
+      <c r="AB47" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>10,8</v>
+      </c>
+      <c r="AC47" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>10,7</v>
+      </c>
+      <c r="AD47" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>10,6</v>
+      </c>
+      <c r="AE47" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>10,5</v>
+      </c>
+      <c r="AF47" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>10,4</v>
+      </c>
+      <c r="AG47" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>10,3</v>
+      </c>
+      <c r="AH47" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>10,2</v>
+      </c>
+      <c r="AI47" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>10,1</v>
+      </c>
+      <c r="AJ47" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>10,0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>9</v>
+      </c>
+      <c r="T48" s="1">
+        <v>9</v>
+      </c>
+      <c r="U48" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>9,15</v>
+      </c>
+      <c r="V48" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>9,14</v>
+      </c>
+      <c r="W48" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>9,13</v>
+      </c>
+      <c r="X48" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>9,12</v>
+      </c>
+      <c r="Y48" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>9,11</v>
+      </c>
+      <c r="Z48" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>9,10</v>
+      </c>
+      <c r="AA48" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>9,9</v>
+      </c>
+      <c r="AB48" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>9,8</v>
+      </c>
+      <c r="AC48" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>9,7</v>
+      </c>
+      <c r="AD48" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>9,6</v>
+      </c>
+      <c r="AE48" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>9,5</v>
+      </c>
+      <c r="AF48" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>9,4</v>
+      </c>
+      <c r="AG48" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>9,3</v>
+      </c>
+      <c r="AH48" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>9,2</v>
+      </c>
+      <c r="AI48" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>9,1</v>
+      </c>
+      <c r="AJ48" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>9,0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>8</v>
+      </c>
+      <c r="T49" s="1">
+        <v>8</v>
+      </c>
+      <c r="U49" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>8,15</v>
+      </c>
+      <c r="V49" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>8,14</v>
+      </c>
+      <c r="W49" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>8,13</v>
+      </c>
+      <c r="X49" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>8,12</v>
+      </c>
+      <c r="Y49" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>8,11</v>
+      </c>
+      <c r="Z49" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>8,10</v>
+      </c>
+      <c r="AA49" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>8,9</v>
+      </c>
+      <c r="AB49" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>8,8</v>
+      </c>
+      <c r="AC49" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>8,7</v>
+      </c>
+      <c r="AD49" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>8,6</v>
+      </c>
+      <c r="AE49" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>8,5</v>
+      </c>
+      <c r="AF49" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>8,4</v>
+      </c>
+      <c r="AG49" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>8,3</v>
+      </c>
+      <c r="AH49" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>8,2</v>
+      </c>
+      <c r="AI49" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>8,1</v>
+      </c>
+      <c r="AJ49" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>8,0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>7</v>
+      </c>
+      <c r="T50" s="1">
+        <v>7</v>
+      </c>
+      <c r="U50" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>7,15</v>
+      </c>
+      <c r="V50" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>7,14</v>
+      </c>
+      <c r="W50" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>7,13</v>
+      </c>
+      <c r="X50" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>7,12</v>
+      </c>
+      <c r="Y50" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>7,11</v>
+      </c>
+      <c r="Z50" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>7,10</v>
+      </c>
+      <c r="AA50" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>7,9</v>
+      </c>
+      <c r="AB50" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>7,8</v>
+      </c>
+      <c r="AC50" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>7,7</v>
+      </c>
+      <c r="AD50" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>7,6</v>
+      </c>
+      <c r="AE50" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>7,5</v>
+      </c>
+      <c r="AF50" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>7,4</v>
+      </c>
+      <c r="AG50" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>7,3</v>
+      </c>
+      <c r="AH50" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>7,2</v>
+      </c>
+      <c r="AI50" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>7,1</v>
+      </c>
+      <c r="AJ50" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>7,0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>6</v>
+      </c>
+      <c r="T51" s="1">
+        <v>6</v>
+      </c>
+      <c r="U51" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>6,15</v>
+      </c>
+      <c r="V51" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>6,14</v>
+      </c>
+      <c r="W51" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>6,13</v>
+      </c>
+      <c r="X51" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>6,12</v>
+      </c>
+      <c r="Y51" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>6,11</v>
+      </c>
+      <c r="Z51" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>6,10</v>
+      </c>
+      <c r="AA51" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>6,9</v>
+      </c>
+      <c r="AB51" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>6,8</v>
+      </c>
+      <c r="AC51" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>6,7</v>
+      </c>
+      <c r="AD51" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>6,6</v>
+      </c>
+      <c r="AE51" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>6,5</v>
+      </c>
+      <c r="AF51" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>6,4</v>
+      </c>
+      <c r="AG51" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>6,3</v>
+      </c>
+      <c r="AH51" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>6,2</v>
+      </c>
+      <c r="AI51" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>6,1</v>
+      </c>
+      <c r="AJ51" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>6,0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>5</v>
+      </c>
+      <c r="T52" s="1">
+        <v>5</v>
+      </c>
+      <c r="U52" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>5,15</v>
+      </c>
+      <c r="V52" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>5,14</v>
+      </c>
+      <c r="W52" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>5,13</v>
+      </c>
+      <c r="X52" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>5,12</v>
+      </c>
+      <c r="Y52" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>5,11</v>
+      </c>
+      <c r="Z52" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>5,10</v>
+      </c>
+      <c r="AA52" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>5,9</v>
+      </c>
+      <c r="AB52" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>5,8</v>
+      </c>
+      <c r="AC52" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>5,7</v>
+      </c>
+      <c r="AD52" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>5,6</v>
+      </c>
+      <c r="AE52" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>5,5</v>
+      </c>
+      <c r="AF52" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>5,4</v>
+      </c>
+      <c r="AG52" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>5,3</v>
+      </c>
+      <c r="AH52" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>5,2</v>
+      </c>
+      <c r="AI52" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>5,1</v>
+      </c>
+      <c r="AJ52" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>5,0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>4</v>
+      </c>
+      <c r="T53" s="1">
+        <v>4</v>
+      </c>
+      <c r="U53" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>4,15</v>
+      </c>
+      <c r="V53" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>4,14</v>
+      </c>
+      <c r="W53" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>4,13</v>
+      </c>
+      <c r="X53" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>4,12</v>
+      </c>
+      <c r="Y53" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>4,11</v>
+      </c>
+      <c r="Z53" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>4,10</v>
+      </c>
+      <c r="AA53" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>4,9</v>
+      </c>
+      <c r="AB53" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>4,8</v>
+      </c>
+      <c r="AC53" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>4,7</v>
+      </c>
+      <c r="AD53" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>4,6</v>
+      </c>
+      <c r="AE53" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>4,5</v>
+      </c>
+      <c r="AF53" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>4,4</v>
+      </c>
+      <c r="AG53" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>4,3</v>
+      </c>
+      <c r="AH53" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>4,2</v>
+      </c>
+      <c r="AI53" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>4,1</v>
+      </c>
+      <c r="AJ53" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>4,0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>3</v>
+      </c>
+      <c r="T54" s="1">
+        <v>3</v>
+      </c>
+      <c r="U54" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>3,15</v>
+      </c>
+      <c r="V54" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>3,14</v>
+      </c>
+      <c r="W54" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>3,13</v>
+      </c>
+      <c r="X54" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>3,12</v>
+      </c>
+      <c r="Y54" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>3,11</v>
+      </c>
+      <c r="Z54" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>3,10</v>
+      </c>
+      <c r="AA54" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>3,9</v>
+      </c>
+      <c r="AB54" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>3,8</v>
+      </c>
+      <c r="AC54" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>3,7</v>
+      </c>
+      <c r="AD54" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>3,6</v>
+      </c>
+      <c r="AE54" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>3,5</v>
+      </c>
+      <c r="AF54" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>3,4</v>
+      </c>
+      <c r="AG54" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>3,3</v>
+      </c>
+      <c r="AH54" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>3,2</v>
+      </c>
+      <c r="AI54" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>3,1</v>
+      </c>
+      <c r="AJ54" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>3,0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>2</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T55" s="1">
+        <v>2</v>
+      </c>
+      <c r="U55" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>2,15</v>
+      </c>
+      <c r="V55" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>2,14</v>
+      </c>
+      <c r="W55" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>2,13</v>
+      </c>
+      <c r="X55" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>2,12</v>
+      </c>
+      <c r="Y55" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>2,11</v>
+      </c>
+      <c r="Z55" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>2,10</v>
+      </c>
+      <c r="AA55" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>2,9</v>
+      </c>
+      <c r="AB55" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="AC55" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>2,7</v>
+      </c>
+      <c r="AD55" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>2,6</v>
+      </c>
+      <c r="AE55" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>2,5</v>
+      </c>
+      <c r="AF55" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>2,4</v>
+      </c>
+      <c r="AG55" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>2,3</v>
+      </c>
+      <c r="AH55" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>2,2</v>
+      </c>
+      <c r="AI55" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>2,1</v>
+      </c>
+      <c r="AJ55" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>2,0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>1</v>
+      </c>
+      <c r="T56" s="1">
+        <v>1</v>
+      </c>
+      <c r="U56" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>1,15</v>
+      </c>
+      <c r="V56" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>1,14</v>
+      </c>
+      <c r="W56" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>1,13</v>
+      </c>
+      <c r="X56" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>1,12</v>
+      </c>
+      <c r="Y56" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>1,11</v>
+      </c>
+      <c r="Z56" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>1,10</v>
+      </c>
+      <c r="AA56" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>1,9</v>
+      </c>
+      <c r="AB56" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>1,8</v>
+      </c>
+      <c r="AC56" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>1,7</v>
+      </c>
+      <c r="AD56" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>1,6</v>
+      </c>
+      <c r="AE56" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>1,5</v>
+      </c>
+      <c r="AF56" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>1,4</v>
+      </c>
+      <c r="AG56" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>1,3</v>
+      </c>
+      <c r="AH56" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>1,2</v>
+      </c>
+      <c r="AI56" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>1,1</v>
+      </c>
+      <c r="AJ56" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>1,0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>0</v>
+      </c>
+      <c r="T57" s="1">
+        <v>0</v>
+      </c>
+      <c r="U57" s="1" t="str">
+        <f t="shared" si="21"/>
+        <v>0,15</v>
+      </c>
+      <c r="V57" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>0,14</v>
+      </c>
+      <c r="W57" s="1" t="str">
+        <f t="shared" si="23"/>
+        <v>0,13</v>
+      </c>
+      <c r="X57" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>0,12</v>
+      </c>
+      <c r="Y57" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v>0,11</v>
+      </c>
+      <c r="Z57" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>0,10</v>
+      </c>
+      <c r="AA57" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v>0,9</v>
+      </c>
+      <c r="AB57" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>0,8</v>
+      </c>
+      <c r="AC57" s="1" t="str">
+        <f t="shared" si="29"/>
+        <v>0,7</v>
+      </c>
+      <c r="AD57" s="1" t="str">
+        <f t="shared" si="30"/>
+        <v>0,6</v>
+      </c>
+      <c r="AE57" s="1" t="str">
+        <f t="shared" si="31"/>
+        <v>0,5</v>
+      </c>
+      <c r="AF57" s="1" t="str">
+        <f t="shared" si="32"/>
+        <v>0,4</v>
+      </c>
+      <c r="AG57" s="1" t="str">
+        <f t="shared" si="33"/>
+        <v>0,3</v>
+      </c>
+      <c r="AH57" s="1" t="str">
+        <f t="shared" si="34"/>
+        <v>0,2</v>
+      </c>
+      <c r="AI57" s="1" t="str">
+        <f t="shared" si="35"/>
+        <v>0,1</v>
+      </c>
+      <c r="AJ57" s="1" t="str">
+        <f t="shared" si="36"/>
+        <v>0,0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>